<commit_message>
merge tim and elise
</commit_message>
<xml_diff>
--- a/logboek-masterproef.xlsx
+++ b/logboek-masterproef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elise\Documents\unif\master\semester2\masterproef\gitProject\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5EB80-1B1D-4A8F-81DD-D6389B035C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0D463-EFD6-42C1-89EB-A12F462E02C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{839A580B-E71F-4714-813D-E450C27D6D09}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="207">
   <si>
     <t>datum</t>
   </si>
@@ -635,6 +635,24 @@
   </si>
   <si>
     <t>experimenten machine learning</t>
+  </si>
+  <si>
+    <t>machine learning onderzoek + sleutelen aan parameters</t>
+  </si>
+  <si>
+    <t>presentatie 1e bachelor + verder machine learning onderzoek</t>
+  </si>
+  <si>
+    <t>forward 180 + cross over meten</t>
+  </si>
+  <si>
+    <t>metingen verwerken + android batch size</t>
+  </si>
+  <si>
+    <t>testen batch size + debuggen</t>
+  </si>
+  <si>
+    <t>workmanager + melding bij te hoge hartslag + tonen mets + verwerken metingen</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8377167A-AB19-4229-9ABE-F6E665BC78B9}">
-  <dimension ref="A1:K140"/>
+  <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="N131" sqref="N131"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1159,7 +1177,7 @@
       </c>
       <c r="F1" s="6">
         <f>SUM(F2:F564)</f>
-        <v>16.319444444444446</v>
+        <v>16.923611111111111</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1680,7 +1698,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" ref="F30:F130" si="1">C30-B30</f>
+        <f t="shared" ref="F30:F136" si="1">C30-B30</f>
         <v>0.19791666666666663</v>
       </c>
     </row>
@@ -3452,7 +3470,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:11">
       <c r="A129" s="1">
         <v>43936</v>
       </c>
@@ -3470,7 +3488,7 @@
         <v>0.16666666666666669</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:11">
       <c r="A130" s="1">
         <v>43936</v>
       </c>
@@ -3488,28 +3506,136 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="131" spans="1:11">
+      <c r="A131" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B131" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C131" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D131" t="s">
+        <v>201</v>
+      </c>
+      <c r="F131" s="2">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B132" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C132" s="2">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D132" t="s">
+        <v>202</v>
+      </c>
+      <c r="F132" s="2">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="1">
+        <v>43938</v>
+      </c>
+      <c r="B133" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D133" t="s">
+        <v>203</v>
+      </c>
+      <c r="F133" s="2">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="1">
+        <v>43938</v>
+      </c>
+      <c r="B134" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C134" s="7">
+        <v>1</v>
+      </c>
+      <c r="D134" t="s">
+        <v>204</v>
+      </c>
+      <c r="F134" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14583333333333337</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
+      <c r="A135" s="1">
+        <v>43939</v>
+      </c>
+      <c r="B135" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C135" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D135" t="s">
+        <v>205</v>
+      </c>
+      <c r="F135" s="2">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="A136" s="1">
+        <v>43939</v>
+      </c>
+      <c r="B136" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C136" s="7">
+        <v>1</v>
+      </c>
       <c r="D136" t="s">
+        <v>206</v>
+      </c>
+      <c r="F136" s="2">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="K137" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
-      <c r="D137" t="s">
+    <row r="138" spans="1:11">
+      <c r="K138" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
-      <c r="D138" t="s">
+    <row r="139" spans="1:11">
+      <c r="K139" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
-      <c r="D139" t="s">
+    <row r="140" spans="1:11">
+      <c r="K140" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
-      <c r="D140" t="s">
+    <row r="141" spans="1:11">
+      <c r="K141" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3523,8 +3649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0632AE7A-6979-4ACF-8714-D96F8B248BF9}">
   <dimension ref="A1:AO60"/>
   <sheetViews>
-    <sheetView topLeftCell="Q20" workbookViewId="0">
-      <selection activeCell="AF34" sqref="AF34"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3661,25 +3787,11 @@
         <v>64</v>
       </c>
       <c r="W3" s="10"/>
-      <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
       <c r="AG3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
-      <c r="AO3" s="15"/>
     </row>
     <row r="4" spans="1:41">
       <c r="A4" s="10" t="s">
@@ -3852,13 +3964,13 @@
       </c>
       <c r="W7" s="10"/>
       <c r="X7" s="8"/>
-      <c r="Y7" s="11"/>
+      <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
-      <c r="AA7" s="11"/>
+      <c r="AA7" s="8"/>
       <c r="AB7" s="8"/>
-      <c r="AC7" s="11"/>
+      <c r="AC7" s="8"/>
       <c r="AD7" s="8"/>
-      <c r="AE7" s="11"/>
+      <c r="AE7" s="8"/>
       <c r="AG7" s="10" t="s">
         <v>56</v>
       </c>

</xml_diff>